<commit_message>
1.0  优化 [Borwser]IE浏览器增加选项参数,增加浏览器初始化和关闭方法,增加单用例计时输出;[Mysql]新增fetchone方法;      新增 [Element]新增imgs入参;新增根据图像特征匹配查找元素方法;删除废弃代码;新增方法:step,double_click,execute_javascript,wait_until_selected,switch_window_by_title,wait_until_alert_and_switch,wait_alert_and_dismiss,wait_alert_and_accept,__draw_click_point,get_ele_by_feature_matching,click_by_featrue_matching;截图增加info参数输出到报告;get_ele_by_img_recognition改为get_ele_by_templ_matching;click_by_img_recognition改为click_by_templ_matching;优化日志输出和样式;           [recognizer]新增match_with_BFMatcher,get_center_of_target_by_feature_matching方法;修改get_dpi;           [HTMLTestRunner]新增返回顶部按钮;新增多线程执行相关方法;移除对python2支持;
</commit_message>
<xml_diff>
--- a/DS/Demo_Web/TestDemo.xlsx
+++ b/DS/Demo_Web/TestDemo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonProject\MyWeb\Upload\DS\Demo_Web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonProject\EasySelenium\DS\Demo_Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787D67FA-B0CA-416D-A4CF-AE92F7A67874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A86297-9542-425D-B821-21834CCC738B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_b" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>参数名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -134,6 +134,18 @@
   </si>
   <si>
     <t>S2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -472,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -486,7 +498,7 @@
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -496,8 +508,20 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -507,8 +531,20 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -518,8 +554,20 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -529,8 +577,20 @@
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -538,6 +598,18 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -545,9 +617,13 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{FA63245C-73E2-4A7D-B3C6-0087B57FDAE2}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{4FDDE476-64F5-4203-9A6F-305E48D2A46C}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{2F0C804B-9CF1-47DE-A4CF-BBA64A1C3A07}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{05DDB2F1-20A1-42D3-BD64-22A6B9FD7E37}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{B406DE63-2391-4DAA-8325-7E81CF0DA3A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -555,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA5231E-0AE1-4699-A1F8-3882763A34DE}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>